<commit_message>
Delete Prometheus MSLA  Assembly.step
</commit_message>
<xml_diff>
--- a/BOM/Prometheus MSLA BOM.xlsx
+++ b/BOM/Prometheus MSLA BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="148">
   <si>
     <t>Category:</t>
   </si>
@@ -67,6 +67,12 @@
     <t>M4x10 HC</t>
   </si>
   <si>
+    <t>*Ball Screw build</t>
+  </si>
+  <si>
+    <t>M4x16 HC</t>
+  </si>
+  <si>
     <t>M4x12 Self Tap</t>
   </si>
   <si>
@@ -79,6 +85,12 @@
     <t>M5x16 HC</t>
   </si>
   <si>
+    <t>M5x35 HC</t>
+  </si>
+  <si>
+    <t>M5x30 HC</t>
+  </si>
+  <si>
     <t>M8x50 ROD</t>
   </si>
   <si>
@@ -88,6 +100,9 @@
     <t>M4 Nut</t>
   </si>
   <si>
+    <t>M5 Nut</t>
+  </si>
+  <si>
     <t>M3 Washer</t>
   </si>
   <si>
@@ -109,6 +124,9 @@
     <t>https://amzn.to/3JTS9Ok</t>
   </si>
   <si>
+    <t xml:space="preserve">*ACME build </t>
+  </si>
+  <si>
     <t>ACME T8 2mm lead 500mm</t>
   </si>
   <si>
@@ -119,6 +137,15 @@
   </si>
   <si>
     <t>https://spool3d.ca/t8-lead-screw-anti-backlash-nut/</t>
+  </si>
+  <si>
+    <t>*Ball Screw Build</t>
+  </si>
+  <si>
+    <t>Ball Screw 450mm 1204</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3Qx7Xuq</t>
   </si>
   <si>
     <t>Linear Rails MGN12H 400mm</t>
@@ -468,7 +495,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -493,6 +520,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF0F1111"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FFFF0000"/>
@@ -525,14 +557,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -542,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -566,8 +598,11 @@
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -780,6 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -901,72 +937,81 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="5">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="5">
-        <v>104.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="5">
-        <v>35.0</v>
+        <v>112.0</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16" s="5">
-        <v>1.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="17">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F17" s="5">
         <v>4.0</v>
       </c>
     </row>
     <row r="18">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C18" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F18" s="5">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F20" s="5">
         <v>4.0</v>
@@ -974,569 +1019,579 @@
     </row>
     <row r="21">
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F21" s="5">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="5">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="C23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F23" s="5">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="C24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="5">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="C26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="C26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="C27" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H27" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30">
       <c r="C30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H30" s="7" t="s">
+      <c r="F31" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31">
-      <c r="C31" s="5" t="s">
+    <row r="32">
+      <c r="A32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H31" s="7" t="s">
+      <c r="F32" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="C33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="34">
       <c r="C34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F35" s="5">
         <v>1.0</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>46</v>
+      <c r="H35" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="36">
       <c r="C36" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F36" s="5">
         <v>1.0</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H37" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="5" t="s">
+      <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39">
       <c r="C39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="F39" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="40">
       <c r="C40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="F40" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="41">
       <c r="C41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="F41" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="42">
       <c r="C42" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="43">
       <c r="C43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="44">
       <c r="C44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="F44" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="45">
       <c r="C45" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H45" s="7" t="s">
+    </row>
+    <row r="46">
+      <c r="C46" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="C46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="F46" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="47">
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="C48" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49">
       <c r="C49" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c r="F49" s="5">
+        <v>2.0</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50">
-      <c r="C50" s="5"/>
-      <c r="F50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
-      <c r="C52" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="C52" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="10"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="C53" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F53" s="5">
+        <v>77</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57">
+      <c r="C57" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F57" s="5">
         <v>2.0</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" s="5"/>
-      <c r="C54" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="C55" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F55" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="F56" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" s="5"/>
-      <c r="C57" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F57" s="5">
-        <v>4.0</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="F58" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="H58" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F58" s="5">
+    </row>
+    <row r="59">
+      <c r="B59" s="5"/>
+      <c r="C59" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" s="5"/>
+      <c r="C61" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="F61" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" s="5"/>
+      <c r="C62" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F62" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F63" s="5">
         <v>36.0</v>
       </c>
-      <c r="H58" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="C59" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F59" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F61" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62">
-      <c r="C62" s="10"/>
-      <c r="F62" s="5"/>
-      <c r="H62" s="5"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
+      <c r="H63" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="64">
-      <c r="C64" s="5" t="s">
-        <v>93</v>
+      <c r="C64" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="F64" s="5">
         <v>2.0</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="F65" s="5">
         <v>1.0</v>
       </c>
+      <c r="H65" s="5"/>
     </row>
     <row r="66">
-      <c r="C66" s="5" t="s">
-        <v>97</v>
+      <c r="A66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="F66" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>98</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="H66" s="5"/>
     </row>
     <row r="67">
-      <c r="C67" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F67" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="C67" s="11"/>
+      <c r="F67" s="5"/>
+      <c r="H67" s="5"/>
     </row>
     <row r="68">
-      <c r="C68" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F68" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H68" s="7" t="s">
+      <c r="A68" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
     </row>
     <row r="69">
       <c r="C69" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F69" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>103</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F70" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
     <row r="71">
-      <c r="A71" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
+      <c r="C71" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F71" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="72">
       <c r="C72" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F72" s="5">
         <v>1.0</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="73">
       <c r="C73" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="F73" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F74" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="76">
-      <c r="C76" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="A76" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
     </row>
     <row r="77">
       <c r="C77" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F77" s="5">
         <v>1.0</v>
       </c>
-      <c r="H77" s="5" t="s">
-        <v>58</v>
+      <c r="H77" s="7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="78">
       <c r="C78" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F78" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1546,64 +1601,69 @@
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
     </row>
+    <row r="81">
+      <c r="C81" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F81" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="82">
-      <c r="A82" s="5" t="s">
-        <v>113</v>
+      <c r="C82" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F82" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="C86" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F86" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="C83" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F83" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
     </row>
     <row r="87">
-      <c r="C87" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F87" s="5">
-        <v>1.0</v>
+      <c r="A87" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="88">
-      <c r="C88" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F88" s="5">
-        <v>1.0</v>
+      <c r="A88" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="89">
-      <c r="C89" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F89" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="C90" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F90" s="5">
-        <v>1.0</v>
+      <c r="A89" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="91">
       <c r="C91" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F91" s="5">
         <v>1.0</v>
@@ -1611,7 +1671,7 @@
     </row>
     <row r="92">
       <c r="C92" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F92" s="5">
         <v>1.0</v>
@@ -1619,7 +1679,7 @@
     </row>
     <row r="93">
       <c r="C93" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F93" s="5">
         <v>1.0</v>
@@ -1627,7 +1687,7 @@
     </row>
     <row r="94">
       <c r="C94" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F94" s="5">
         <v>1.0</v>
@@ -1635,7 +1695,7 @@
     </row>
     <row r="95">
       <c r="C95" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F95" s="5">
         <v>1.0</v>
@@ -1643,7 +1703,7 @@
     </row>
     <row r="96">
       <c r="C96" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F96" s="5">
         <v>1.0</v>
@@ -1651,7 +1711,7 @@
     </row>
     <row r="97">
       <c r="C97" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F97" s="5">
         <v>1.0</v>
@@ -1659,7 +1719,7 @@
     </row>
     <row r="98">
       <c r="C98" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F98" s="5">
         <v>1.0</v>
@@ -1667,7 +1727,7 @@
     </row>
     <row r="99">
       <c r="C99" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F99" s="5">
         <v>1.0</v>
@@ -1675,7 +1735,7 @@
     </row>
     <row r="100">
       <c r="C100" s="5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F100" s="5">
         <v>1.0</v>
@@ -1683,7 +1743,7 @@
     </row>
     <row r="101">
       <c r="C101" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F101" s="5">
         <v>1.0</v>
@@ -1691,7 +1751,7 @@
     </row>
     <row r="102">
       <c r="C102" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F102" s="5">
         <v>1.0</v>
@@ -1699,7 +1759,7 @@
     </row>
     <row r="103">
       <c r="C103" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F103" s="5">
         <v>1.0</v>
@@ -1707,7 +1767,7 @@
     </row>
     <row r="104">
       <c r="C104" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F104" s="5">
         <v>1.0</v>
@@ -1715,7 +1775,7 @@
     </row>
     <row r="105">
       <c r="C105" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F105" s="5">
         <v>1.0</v>
@@ -1723,7 +1783,7 @@
     </row>
     <row r="106">
       <c r="C106" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F106" s="5">
         <v>1.0</v>
@@ -1731,15 +1791,55 @@
     </row>
     <row r="107">
       <c r="C107" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F107" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F108" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F109" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F110" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F111" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F112" s="5">
         <v>2.0</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="5" t="s">
-        <v>138</v>
+    <row r="114">
+      <c r="A114" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1748,38 +1848,42 @@
     <hyperlink r:id="rId2" ref="H4"/>
     <hyperlink r:id="rId3" ref="H5"/>
     <hyperlink r:id="rId4" ref="H6"/>
-    <hyperlink r:id="rId5" ref="H26"/>
-    <hyperlink r:id="rId6" ref="H27"/>
-    <hyperlink r:id="rId7" ref="H28"/>
-    <hyperlink r:id="rId8" ref="H29"/>
-    <hyperlink r:id="rId9" ref="H30"/>
-    <hyperlink r:id="rId10" ref="H31"/>
-    <hyperlink r:id="rId11" ref="H34"/>
-    <hyperlink r:id="rId12" ref="H35"/>
-    <hyperlink r:id="rId13" ref="H36"/>
-    <hyperlink r:id="rId14" ref="H37"/>
-    <hyperlink r:id="rId15" ref="H38"/>
-    <hyperlink r:id="rId16" ref="H39"/>
-    <hyperlink r:id="rId17" ref="H40"/>
-    <hyperlink r:id="rId18" ref="H43"/>
-    <hyperlink r:id="rId19" ref="H44"/>
-    <hyperlink r:id="rId20" ref="H45"/>
-    <hyperlink r:id="rId21" ref="H48"/>
-    <hyperlink r:id="rId22" ref="H49"/>
-    <hyperlink r:id="rId23" ref="H52"/>
-    <hyperlink r:id="rId24" ref="H53"/>
-    <hyperlink r:id="rId25" ref="H54"/>
-    <hyperlink r:id="rId26" ref="H55"/>
-    <hyperlink r:id="rId27" ref="H56"/>
-    <hyperlink r:id="rId28" ref="H57"/>
-    <hyperlink r:id="rId29" ref="H58"/>
-    <hyperlink r:id="rId30" ref="H59"/>
+    <hyperlink r:id="rId5" ref="H30"/>
+    <hyperlink r:id="rId6" ref="H31"/>
+    <hyperlink r:id="rId7" ref="H32"/>
+    <hyperlink r:id="rId8" ref="H33"/>
+    <hyperlink r:id="rId9" ref="H34"/>
+    <hyperlink r:id="rId10" ref="H35"/>
+    <hyperlink r:id="rId11" ref="H36"/>
+    <hyperlink r:id="rId12" ref="H39"/>
+    <hyperlink r:id="rId13" ref="H40"/>
+    <hyperlink r:id="rId14" ref="H41"/>
+    <hyperlink r:id="rId15" ref="H42"/>
+    <hyperlink r:id="rId16" ref="H43"/>
+    <hyperlink r:id="rId17" ref="H44"/>
+    <hyperlink r:id="rId18" ref="H45"/>
+    <hyperlink r:id="rId19" ref="H48"/>
+    <hyperlink r:id="rId20" ref="H49"/>
+    <hyperlink r:id="rId21" ref="H50"/>
+    <hyperlink r:id="rId22" ref="H53"/>
+    <hyperlink r:id="rId23" ref="H54"/>
+    <hyperlink r:id="rId24" ref="H57"/>
+    <hyperlink r:id="rId25" ref="H58"/>
+    <hyperlink r:id="rId26" ref="H59"/>
+    <hyperlink r:id="rId27" ref="H60"/>
+    <hyperlink r:id="rId28" ref="H61"/>
+    <hyperlink r:id="rId29" ref="H62"/>
+    <hyperlink r:id="rId30" ref="H63"/>
     <hyperlink r:id="rId31" ref="H64"/>
-    <hyperlink r:id="rId32" ref="H66"/>
-    <hyperlink r:id="rId33" ref="H68"/>
-    <hyperlink r:id="rId34" ref="H69"/>
-    <hyperlink r:id="rId35" ref="H72"/>
+    <hyperlink r:id="rId32" ref="H69"/>
+    <hyperlink r:id="rId33" ref="H71"/>
+    <hyperlink r:id="rId34" ref="H73"/>
+    <hyperlink r:id="rId35" ref="H74"/>
+    <hyperlink r:id="rId36" ref="H77"/>
   </hyperlinks>
-  <drawing r:id="rId36"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>